<commit_message>
Statistik für A6 hinzufügen. Präsentation vorbereiten.
</commit_message>
<xml_diff>
--- a/Projekt 1/Aufgabe6/Statistik.xlsx
+++ b/Projekt 1/Aufgabe6/Statistik.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="22">
   <si>
     <t>l</t>
   </si>
@@ -81,6 +81,15 @@
   </si>
   <si>
     <t>E(32)</t>
+  </si>
+  <si>
+    <t>S(1)</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A6</t>
   </si>
 </sst>
 </file>
@@ -261,7 +270,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
@@ -277,6 +286,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Ergebnis" xfId="1" builtinId="25"/>
@@ -592,15 +602,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:U13"/>
+  <dimension ref="B3:U38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S40" sqref="S40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G3">
         <v>2</v>
       </c>
@@ -617,7 +627,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
@@ -676,7 +689,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="3:21" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:21" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C5">
         <v>1</v>
       </c>
@@ -747,7 +760,7 @@
         <v>2.1964856230031948E-3</v>
       </c>
     </row>
-    <row r="6" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>2</v>
       </c>
@@ -818,7 +831,7 @@
         <v>1.4784946236559141E-3</v>
       </c>
     </row>
-    <row r="7" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>3</v>
       </c>
@@ -889,7 +902,7 @@
         <v>8.8131609870740308E-4</v>
       </c>
     </row>
-    <row r="8" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>4</v>
       </c>
@@ -960,7 +973,7 @@
         <v>4.2998224589436306E-4</v>
       </c>
     </row>
-    <row r="9" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>5</v>
       </c>
@@ -1031,7 +1044,7 @@
         <v>6.227926337033301E-4</v>
       </c>
     </row>
-    <row r="10" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C10">
         <v>6</v>
       </c>
@@ -1102,7 +1115,7 @@
         <v>2.0790816326530614E-3</v>
       </c>
     </row>
-    <row r="11" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C11">
         <v>7</v>
       </c>
@@ -1173,7 +1186,7 @@
         <v>8.353232916972814E-3</v>
       </c>
     </row>
-    <row r="12" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C12">
         <v>8</v>
       </c>
@@ -1244,7 +1257,7 @@
         <v>4.0627684586517158E-2</v>
       </c>
     </row>
-    <row r="13" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C13">
         <v>9</v>
       </c>
@@ -1313,6 +1326,1265 @@
       <c r="U13" s="10">
         <f t="shared" si="11"/>
         <v>0.38989707475622964</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="T16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="U16" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="3:21" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <f>2^C17-1</f>
+        <v>1</v>
+      </c>
+      <c r="E17" s="6">
+        <f>D17*D17</f>
+        <v>1</v>
+      </c>
+      <c r="F17" s="13">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="G17" s="5">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="H17" s="6">
+        <f>$F17/G17</f>
+        <v>1</v>
+      </c>
+      <c r="I17" s="7">
+        <f>H17/G$3</f>
+        <v>0.5</v>
+      </c>
+      <c r="J17" s="5">
+        <v>3.7000000000000002E-3</v>
+      </c>
+      <c r="K17" s="6">
+        <f>$F17/J17</f>
+        <v>0.97297297297297292</v>
+      </c>
+      <c r="L17" s="7">
+        <f>K17/J$3</f>
+        <v>0.24324324324324323</v>
+      </c>
+      <c r="M17" s="5">
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="N17" s="6">
+        <f>$F17/M17</f>
+        <v>0.37894736842105264</v>
+      </c>
+      <c r="O17" s="7">
+        <f>N17/M$3</f>
+        <v>4.736842105263158E-2</v>
+      </c>
+      <c r="P17" s="5">
+        <v>1.49E-2</v>
+      </c>
+      <c r="Q17" s="6">
+        <f>$F17/P17</f>
+        <v>0.24161073825503354</v>
+      </c>
+      <c r="R17" s="7">
+        <f>Q17/P$3</f>
+        <v>1.5100671140939596E-2</v>
+      </c>
+      <c r="S17" s="5">
+        <v>2.1499999999999998E-2</v>
+      </c>
+      <c r="T17" s="6">
+        <f>$F17/S17</f>
+        <v>0.16744186046511628</v>
+      </c>
+      <c r="U17" s="7">
+        <f>T17/S$3</f>
+        <v>5.2325581395348836E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ref="D18:D25" si="12">2^C18-1</f>
+        <v>3</v>
+      </c>
+      <c r="E18" s="6">
+        <f t="shared" ref="E18:E25" si="13">D18*D18</f>
+        <v>9</v>
+      </c>
+      <c r="F18" s="13">
+        <v>3.3E-3</v>
+      </c>
+      <c r="G18" s="5">
+        <v>3.3999999999999998E-3</v>
+      </c>
+      <c r="H18" s="6">
+        <f t="shared" ref="H18:H25" si="14">$F18/G18</f>
+        <v>0.97058823529411764</v>
+      </c>
+      <c r="I18" s="7">
+        <f t="shared" ref="I18:I25" si="15">H18/G$3</f>
+        <v>0.48529411764705882</v>
+      </c>
+      <c r="J18" s="5">
+        <v>3.3E-3</v>
+      </c>
+      <c r="K18" s="6">
+        <f t="shared" ref="K18:K25" si="16">$F18/J18</f>
+        <v>1</v>
+      </c>
+      <c r="L18" s="7">
+        <f t="shared" ref="L18:L25" si="17">K18/J$3</f>
+        <v>0.25</v>
+      </c>
+      <c r="M18" s="5">
+        <v>1.2800000000000001E-2</v>
+      </c>
+      <c r="N18" s="6">
+        <f t="shared" ref="N18:N25" si="18">$F18/M18</f>
+        <v>0.2578125</v>
+      </c>
+      <c r="O18" s="7">
+        <f t="shared" ref="O18:O25" si="19">N18/M$3</f>
+        <v>3.22265625E-2</v>
+      </c>
+      <c r="P18" s="5">
+        <v>5.5800000000000002E-2</v>
+      </c>
+      <c r="Q18" s="6">
+        <f t="shared" ref="Q18:Q25" si="20">$F18/P18</f>
+        <v>5.9139784946236555E-2</v>
+      </c>
+      <c r="R18" s="7">
+        <f t="shared" ref="R18:R25" si="21">Q18/P$3</f>
+        <v>3.6962365591397847E-3</v>
+      </c>
+      <c r="S18" s="5">
+        <v>0.11559999999999999</v>
+      </c>
+      <c r="T18" s="6">
+        <f t="shared" ref="T18:T25" si="22">$F18/S18</f>
+        <v>2.8546712802768166E-2</v>
+      </c>
+      <c r="U18" s="7">
+        <f t="shared" ref="U18:U25" si="23">T18/S$3</f>
+        <v>8.920847750865052E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="12"/>
+        <v>7</v>
+      </c>
+      <c r="E19" s="6">
+        <f t="shared" si="13"/>
+        <v>49</v>
+      </c>
+      <c r="F19" s="13">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="G19" s="5">
+        <v>3.0999999999999999E-3</v>
+      </c>
+      <c r="H19" s="6">
+        <f t="shared" si="14"/>
+        <v>0.87096774193548399</v>
+      </c>
+      <c r="I19" s="7">
+        <f t="shared" si="15"/>
+        <v>0.43548387096774199</v>
+      </c>
+      <c r="J19" s="5">
+        <v>3.3E-3</v>
+      </c>
+      <c r="K19" s="6">
+        <f t="shared" si="16"/>
+        <v>0.81818181818181823</v>
+      </c>
+      <c r="L19" s="7">
+        <f t="shared" si="17"/>
+        <v>0.20454545454545456</v>
+      </c>
+      <c r="M19" s="5">
+        <v>8.3999999999999995E-3</v>
+      </c>
+      <c r="N19" s="6">
+        <f t="shared" si="18"/>
+        <v>0.32142857142857145</v>
+      </c>
+      <c r="O19" s="7">
+        <f t="shared" si="19"/>
+        <v>4.0178571428571432E-2</v>
+      </c>
+      <c r="P19" s="5">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="Q19" s="6">
+        <f t="shared" si="20"/>
+        <v>2.9347826086956522E-2</v>
+      </c>
+      <c r="R19" s="7">
+        <f t="shared" si="21"/>
+        <v>1.8342391304347826E-3</v>
+      </c>
+      <c r="S19" s="5">
+        <v>0.28710000000000002</v>
+      </c>
+      <c r="T19" s="6">
+        <f t="shared" si="22"/>
+        <v>9.4043887147335428E-3</v>
+      </c>
+      <c r="U19" s="7">
+        <f t="shared" si="23"/>
+        <v>2.9388714733542321E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="12"/>
+        <v>15</v>
+      </c>
+      <c r="E20" s="6">
+        <f t="shared" si="13"/>
+        <v>225</v>
+      </c>
+      <c r="F20" s="13">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="G20" s="5">
+        <v>5.7999999999999996E-3</v>
+      </c>
+      <c r="H20" s="6">
+        <f t="shared" si="14"/>
+        <v>0.93103448275862077</v>
+      </c>
+      <c r="I20" s="7">
+        <f t="shared" si="15"/>
+        <v>0.46551724137931039</v>
+      </c>
+      <c r="J20" s="5">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="K20" s="6">
+        <f t="shared" si="16"/>
+        <v>0.80597014925373134</v>
+      </c>
+      <c r="L20" s="7">
+        <f t="shared" si="17"/>
+        <v>0.20149253731343283</v>
+      </c>
+      <c r="M20" s="5">
+        <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="N20" s="6">
+        <f t="shared" si="18"/>
+        <v>0.34177215189873417</v>
+      </c>
+      <c r="O20" s="7">
+        <f t="shared" si="19"/>
+        <v>4.2721518987341771E-2</v>
+      </c>
+      <c r="P20" s="5">
+        <v>0.18659999999999999</v>
+      </c>
+      <c r="Q20" s="6">
+        <f t="shared" si="20"/>
+        <v>2.8938906752411578E-2</v>
+      </c>
+      <c r="R20" s="7">
+        <f t="shared" si="21"/>
+        <v>1.8086816720257236E-3</v>
+      </c>
+      <c r="S20" s="5">
+        <v>0.66110000000000002</v>
+      </c>
+      <c r="T20" s="6">
+        <f t="shared" si="22"/>
+        <v>8.1682045076387835E-3</v>
+      </c>
+      <c r="U20" s="7">
+        <f t="shared" si="23"/>
+        <v>2.5525639086371199E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="12"/>
+        <v>31</v>
+      </c>
+      <c r="E21" s="6">
+        <f t="shared" si="13"/>
+        <v>961</v>
+      </c>
+      <c r="F21" s="13">
+        <v>3.1699999999999999E-2</v>
+      </c>
+      <c r="G21" s="5">
+        <v>2.4500000000000001E-2</v>
+      </c>
+      <c r="H21" s="6">
+        <f t="shared" si="14"/>
+        <v>1.2938775510204081</v>
+      </c>
+      <c r="I21" s="7">
+        <f t="shared" si="15"/>
+        <v>0.64693877551020407</v>
+      </c>
+      <c r="J21" s="5">
+        <v>2.3900000000000001E-2</v>
+      </c>
+      <c r="K21" s="6">
+        <f t="shared" si="16"/>
+        <v>1.3263598326359831</v>
+      </c>
+      <c r="L21" s="7">
+        <f t="shared" si="17"/>
+        <v>0.33158995815899578</v>
+      </c>
+      <c r="M21" s="5">
+        <v>2.98E-2</v>
+      </c>
+      <c r="N21" s="6">
+        <f t="shared" si="18"/>
+        <v>1.0637583892617448</v>
+      </c>
+      <c r="O21" s="7">
+        <f t="shared" si="19"/>
+        <v>0.1329697986577181</v>
+      </c>
+      <c r="P21" s="5">
+        <v>0.1986</v>
+      </c>
+      <c r="Q21" s="6">
+        <f t="shared" si="20"/>
+        <v>0.15961732124874117</v>
+      </c>
+      <c r="R21" s="7">
+        <f t="shared" si="21"/>
+        <v>9.9760825780463233E-3</v>
+      </c>
+      <c r="S21" s="5">
+        <v>1.3776999999999999</v>
+      </c>
+      <c r="T21" s="6">
+        <f t="shared" si="22"/>
+        <v>2.3009363431806634E-2</v>
+      </c>
+      <c r="U21" s="7">
+        <f t="shared" si="23"/>
+        <v>7.190426072439573E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>6</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="12"/>
+        <v>63</v>
+      </c>
+      <c r="E22" s="6">
+        <f t="shared" si="13"/>
+        <v>3969</v>
+      </c>
+      <c r="F22" s="13">
+        <v>0.3296</v>
+      </c>
+      <c r="G22" s="5">
+        <v>0.20380000000000001</v>
+      </c>
+      <c r="H22" s="6">
+        <f t="shared" si="14"/>
+        <v>1.6172718351324828</v>
+      </c>
+      <c r="I22" s="7">
+        <f t="shared" si="15"/>
+        <v>0.80863591756624142</v>
+      </c>
+      <c r="J22" s="5">
+        <v>0.16020000000000001</v>
+      </c>
+      <c r="K22" s="6">
+        <f t="shared" si="16"/>
+        <v>2.0574282147315852</v>
+      </c>
+      <c r="L22" s="7">
+        <f t="shared" si="17"/>
+        <v>0.5143570536828963</v>
+      </c>
+      <c r="M22" s="5">
+        <v>0.1633</v>
+      </c>
+      <c r="N22" s="6">
+        <f t="shared" si="18"/>
+        <v>2.01837109614207</v>
+      </c>
+      <c r="O22" s="7">
+        <f t="shared" si="19"/>
+        <v>0.25229638701775875</v>
+      </c>
+      <c r="P22" s="5">
+        <v>0.43759999999999999</v>
+      </c>
+      <c r="Q22" s="6">
+        <f t="shared" si="20"/>
+        <v>0.75319926873857412</v>
+      </c>
+      <c r="R22" s="7">
+        <f t="shared" si="21"/>
+        <v>4.7074954296160883E-2</v>
+      </c>
+      <c r="S22" s="5">
+        <v>2.9317000000000002</v>
+      </c>
+      <c r="T22" s="6">
+        <f t="shared" si="22"/>
+        <v>0.11242623733669883</v>
+      </c>
+      <c r="U22" s="7">
+        <f t="shared" si="23"/>
+        <v>3.5133199167718386E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <v>7</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="12"/>
+        <v>127</v>
+      </c>
+      <c r="E23" s="6">
+        <f t="shared" si="13"/>
+        <v>16129</v>
+      </c>
+      <c r="F23" s="13">
+        <v>4.1139999999999999</v>
+      </c>
+      <c r="G23" s="5">
+        <v>2.246</v>
+      </c>
+      <c r="H23" s="6">
+        <f t="shared" si="14"/>
+        <v>1.8317008014247551</v>
+      </c>
+      <c r="I23" s="7">
+        <f t="shared" si="15"/>
+        <v>0.91585040071237755</v>
+      </c>
+      <c r="J23" s="5">
+        <v>1.413</v>
+      </c>
+      <c r="K23" s="6">
+        <f t="shared" si="16"/>
+        <v>2.9115357395612169</v>
+      </c>
+      <c r="L23" s="7">
+        <f t="shared" si="17"/>
+        <v>0.72788393489030423</v>
+      </c>
+      <c r="M23" s="5">
+        <v>1.1160000000000001</v>
+      </c>
+      <c r="N23" s="6">
+        <f t="shared" si="18"/>
+        <v>3.6863799283154117</v>
+      </c>
+      <c r="O23" s="7">
+        <f t="shared" si="19"/>
+        <v>0.46079749103942647</v>
+      </c>
+      <c r="P23" s="5">
+        <v>1.7629999999999999</v>
+      </c>
+      <c r="Q23" s="6">
+        <f t="shared" si="20"/>
+        <v>2.3335224049914918</v>
+      </c>
+      <c r="R23" s="7">
+        <f t="shared" si="21"/>
+        <v>0.14584515031196824</v>
+      </c>
+      <c r="S23" s="5">
+        <v>3.3519999999999999</v>
+      </c>
+      <c r="T23" s="6">
+        <f t="shared" si="22"/>
+        <v>1.2273269689737469</v>
+      </c>
+      <c r="U23" s="7">
+        <f t="shared" si="23"/>
+        <v>3.8353967780429592E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="12"/>
+        <v>255</v>
+      </c>
+      <c r="E24" s="6">
+        <f t="shared" si="13"/>
+        <v>65025</v>
+      </c>
+      <c r="F24" s="13">
+        <v>51.338000000000001</v>
+      </c>
+      <c r="G24" s="5">
+        <v>27.56</v>
+      </c>
+      <c r="H24" s="6">
+        <f t="shared" si="14"/>
+        <v>1.8627721335268506</v>
+      </c>
+      <c r="I24" s="7">
+        <f t="shared" si="15"/>
+        <v>0.93138606676342528</v>
+      </c>
+      <c r="J24" s="5">
+        <v>15.316000000000001</v>
+      </c>
+      <c r="K24" s="6">
+        <f t="shared" si="16"/>
+        <v>3.3519195612431445</v>
+      </c>
+      <c r="L24" s="7">
+        <f t="shared" si="17"/>
+        <v>0.83797989031078612</v>
+      </c>
+      <c r="M24" s="5">
+        <v>11.2</v>
+      </c>
+      <c r="N24" s="6">
+        <f t="shared" si="18"/>
+        <v>4.5837500000000002</v>
+      </c>
+      <c r="O24" s="7">
+        <f t="shared" si="19"/>
+        <v>0.57296875000000003</v>
+      </c>
+      <c r="P24" s="5">
+        <v>9.3729999999999993</v>
+      </c>
+      <c r="Q24" s="6">
+        <f t="shared" si="20"/>
+        <v>5.4772218073188954</v>
+      </c>
+      <c r="R24" s="7">
+        <f t="shared" si="21"/>
+        <v>0.34232636295743096</v>
+      </c>
+      <c r="S24" s="5">
+        <v>8.9589999999999996</v>
+      </c>
+      <c r="T24" s="6">
+        <f t="shared" si="22"/>
+        <v>5.7303270454291777</v>
+      </c>
+      <c r="U24" s="7">
+        <f t="shared" si="23"/>
+        <v>0.1790727201696618</v>
+      </c>
+    </row>
+    <row r="25" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25">
+        <v>9</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="12"/>
+        <v>511</v>
+      </c>
+      <c r="E25" s="6">
+        <f t="shared" si="13"/>
+        <v>261121</v>
+      </c>
+      <c r="F25" s="14">
+        <v>635.26599999999996</v>
+      </c>
+      <c r="G25" s="8">
+        <v>347.36799999999999</v>
+      </c>
+      <c r="H25" s="9">
+        <f t="shared" si="14"/>
+        <v>1.8287982773312452</v>
+      </c>
+      <c r="I25" s="10">
+        <f t="shared" si="15"/>
+        <v>0.91439913866562261</v>
+      </c>
+      <c r="J25" s="8">
+        <v>188.80199999999999</v>
+      </c>
+      <c r="K25" s="9">
+        <f t="shared" si="16"/>
+        <v>3.3647207127043144</v>
+      </c>
+      <c r="L25" s="10">
+        <f t="shared" si="17"/>
+        <v>0.8411801781760786</v>
+      </c>
+      <c r="M25" s="8">
+        <v>115.59699999999999</v>
+      </c>
+      <c r="N25" s="9">
+        <f t="shared" si="18"/>
+        <v>5.4955232402224974</v>
+      </c>
+      <c r="O25" s="10">
+        <f t="shared" si="19"/>
+        <v>0.68694040502781217</v>
+      </c>
+      <c r="P25" s="8">
+        <v>76.593000000000004</v>
+      </c>
+      <c r="Q25" s="9">
+        <f t="shared" si="20"/>
+        <v>8.2940477589335835</v>
+      </c>
+      <c r="R25" s="10">
+        <f t="shared" si="21"/>
+        <v>0.51837798493334897</v>
+      </c>
+      <c r="S25" s="8">
+        <v>69.953000000000003</v>
+      </c>
+      <c r="T25" s="9">
+        <f t="shared" si="22"/>
+        <v>9.0813260331937151</v>
+      </c>
+      <c r="U25" s="10">
+        <f t="shared" si="23"/>
+        <v>0.2837914385373036</v>
+      </c>
+    </row>
+    <row r="29" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H29" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J29" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K29" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="L29" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="M29" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="N29" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="O29" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="P29" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="3:21" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <f>2^C30-1</f>
+        <v>1</v>
+      </c>
+      <c r="E30" s="6">
+        <f>D30*D30</f>
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <f>F17/F5</f>
+        <v>1.6363636363636362</v>
+      </c>
+      <c r="G30">
+        <f>G17/G5</f>
+        <v>1.5</v>
+      </c>
+      <c r="H30">
+        <f>G30/2</f>
+        <v>0.75</v>
+      </c>
+      <c r="I30">
+        <f>J17/J5</f>
+        <v>1.2758620689655173</v>
+      </c>
+      <c r="J30">
+        <f>I30/2</f>
+        <v>0.63793103448275867</v>
+      </c>
+      <c r="K30">
+        <f>M17/M5</f>
+        <v>1.0439560439560438</v>
+      </c>
+      <c r="L30">
+        <f>K30/2</f>
+        <v>0.5219780219780219</v>
+      </c>
+      <c r="M30">
+        <f>P17/P5</f>
+        <v>0.70283018867924529</v>
+      </c>
+      <c r="N30">
+        <f>M30/2</f>
+        <v>0.35141509433962265</v>
+      </c>
+      <c r="O30">
+        <f>S17/S5</f>
+        <v>0.6869009584664536</v>
+      </c>
+      <c r="P30">
+        <f>O30/2</f>
+        <v>0.3434504792332268</v>
+      </c>
+    </row>
+    <row r="31" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <f t="shared" ref="D31:D38" si="24">2^C31-1</f>
+        <v>3</v>
+      </c>
+      <c r="E31" s="6">
+        <f t="shared" ref="E31:E38" si="25">D31*D31</f>
+        <v>9</v>
+      </c>
+      <c r="F31">
+        <f>F18/F6</f>
+        <v>1.5</v>
+      </c>
+      <c r="G31">
+        <f t="shared" ref="G31:G38" si="26">G18/G6</f>
+        <v>1.3599999999999999</v>
+      </c>
+      <c r="H31">
+        <f t="shared" ref="H31:H38" si="27">G31/2</f>
+        <v>0.67999999999999994</v>
+      </c>
+      <c r="I31">
+        <f t="shared" ref="I31:I38" si="28">J18/J6</f>
+        <v>1.1379310344827587</v>
+      </c>
+      <c r="J31">
+        <f t="shared" ref="J31:J38" si="29">I31/2</f>
+        <v>0.56896551724137934</v>
+      </c>
+      <c r="K31">
+        <f t="shared" ref="K31:K38" si="30">M18/M6</f>
+        <v>1.9393939393939394</v>
+      </c>
+      <c r="L31">
+        <f t="shared" ref="L31:L38" si="31">K31/2</f>
+        <v>0.96969696969696972</v>
+      </c>
+      <c r="M31">
+        <f t="shared" ref="M31:M38" si="32">P18/P6</f>
+        <v>2.0144404332129966</v>
+      </c>
+      <c r="N31">
+        <f t="shared" ref="N31:N38" si="33">M31/2</f>
+        <v>1.0072202166064983</v>
+      </c>
+      <c r="O31">
+        <f t="shared" ref="O31:O38" si="34">S18/S6</f>
+        <v>2.4860215053763439</v>
+      </c>
+      <c r="P31">
+        <f t="shared" ref="P31:P38" si="35">O31/2</f>
+        <v>1.243010752688172</v>
+      </c>
+    </row>
+    <row r="32" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="24"/>
+        <v>7</v>
+      </c>
+      <c r="E32" s="6">
+        <f t="shared" si="25"/>
+        <v>49</v>
+      </c>
+      <c r="F32">
+        <f>F19/F7</f>
+        <v>1.1250000000000002</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="26"/>
+        <v>1.1923076923076923</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="27"/>
+        <v>0.59615384615384615</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="28"/>
+        <v>1.2222222222222221</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="29"/>
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="30"/>
+        <v>0.8484848484848484</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="31"/>
+        <v>0.4242424242424242</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="32"/>
+        <v>2.227602905569007</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="33"/>
+        <v>1.1138014527845035</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="34"/>
+        <v>3.3736780258519392</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="35"/>
+        <v>1.6868390129259696</v>
+      </c>
+    </row>
+    <row r="33" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="24"/>
+        <v>15</v>
+      </c>
+      <c r="E33" s="6">
+        <f t="shared" si="25"/>
+        <v>225</v>
+      </c>
+      <c r="F33">
+        <f>F20/F8</f>
+        <v>1.741935483870968</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="26"/>
+        <v>1.8124999999999998</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="27"/>
+        <v>0.90624999999999989</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="28"/>
+        <v>2.09375</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="29"/>
+        <v>1.046875</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="30"/>
+        <v>1.1205673758865249</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="31"/>
+        <v>0.56028368794326244</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="32"/>
+        <v>2.4424083769633507</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="33"/>
+        <v>1.2212041884816753</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="34"/>
+        <v>2.9343098091433646</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="35"/>
+        <v>1.4671549045716823</v>
+      </c>
+    </row>
+    <row r="34" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C34">
+        <v>5</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="24"/>
+        <v>31</v>
+      </c>
+      <c r="E34" s="6">
+        <f t="shared" si="25"/>
+        <v>961</v>
+      </c>
+      <c r="F34">
+        <f>F21/F9</f>
+        <v>4.0126582278481004</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="26"/>
+        <v>3.7121212121212124</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="27"/>
+        <v>1.8560606060606062</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="28"/>
+        <v>4.3454545454545457</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="29"/>
+        <v>2.1727272727272728</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="30"/>
+        <v>1.6021505376344087</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="31"/>
+        <v>0.80107526881720437</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="32"/>
+        <v>1.4360086767895879</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="33"/>
+        <v>0.71800433839479394</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="34"/>
+        <v>3.4755297679112007</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="35"/>
+        <v>1.7377648839556004</v>
+      </c>
+    </row>
+    <row r="35" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C35">
+        <v>6</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="24"/>
+        <v>63</v>
+      </c>
+      <c r="E35" s="6">
+        <f t="shared" si="25"/>
+        <v>3969</v>
+      </c>
+      <c r="F35">
+        <f>F22/F10</f>
+        <v>6.740286298568507</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="26"/>
+        <v>6.9794520547945211</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="27"/>
+        <v>3.4897260273972606</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="28"/>
+        <v>9</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="29"/>
+        <v>4.5</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="30"/>
+        <v>6.8326359832635983</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="31"/>
+        <v>3.4163179916317992</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="32"/>
+        <v>2.3413590155163186</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="33"/>
+        <v>1.1706795077581593</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="34"/>
+        <v>3.9887074829931977</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="35"/>
+        <v>1.9943537414965988</v>
+      </c>
+    </row>
+    <row r="36" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C36">
+        <v>7</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="24"/>
+        <v>127</v>
+      </c>
+      <c r="E36" s="6">
+        <f t="shared" si="25"/>
+        <v>16129</v>
+      </c>
+      <c r="F36">
+        <f>F23/F11</f>
+        <v>11.308411214953271</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="26"/>
+        <v>10.950755728912725</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="27"/>
+        <v>5.4753778644563624</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="28"/>
+        <v>12.798913043478262</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="29"/>
+        <v>6.3994565217391308</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="30"/>
+        <v>13.41346153846154</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="31"/>
+        <v>6.7067307692307701</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="32"/>
+        <v>4.9232058084333987</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="33"/>
+        <v>2.4616029042166994</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="34"/>
+        <v>2.4628949301983836</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="35"/>
+        <v>1.2314474650991918</v>
+      </c>
+    </row>
+    <row r="37" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C37">
+        <v>8</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="24"/>
+        <v>255</v>
+      </c>
+      <c r="E37" s="6">
+        <f t="shared" si="25"/>
+        <v>65025</v>
+      </c>
+      <c r="F37">
+        <f>F24/F12</f>
+        <v>17.854211587952982</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="26"/>
+        <v>16.539638720518514</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="27"/>
+        <v>8.2698193602592571</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="28"/>
+        <v>18.357904830396741</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="29"/>
+        <v>9.1789524151983706</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="30"/>
+        <v>24.018871970834226</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="31"/>
+        <v>12.009435985417113</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="32"/>
+        <v>16.833692528735632</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="33"/>
+        <v>8.4168462643678161</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="34"/>
+        <v>4.0507302075326672</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="35"/>
+        <v>2.0253651037663336</v>
+      </c>
+    </row>
+    <row r="38" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C38">
+        <v>9</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="24"/>
+        <v>511</v>
+      </c>
+      <c r="E38" s="6">
+        <f t="shared" si="25"/>
+        <v>261121</v>
+      </c>
+      <c r="F38">
+        <f>F25/F13</f>
+        <v>27.581886071552621</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="26"/>
+        <v>25.872784150156413</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="27"/>
+        <v>12.936392075078206</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="28"/>
+        <v>27.291413703382478</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="29"/>
+        <v>13.645706851691239</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="30"/>
+        <v>31.540791268758525</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="31"/>
+        <v>15.770395634379263</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="32"/>
+        <v>39.501289324394016</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="33"/>
+        <v>19.750644662197008</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="34"/>
+        <v>37.894366197183096</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="35"/>
+        <v>18.947183098591548</v>
       </c>
     </row>
   </sheetData>

</xml_diff>